<commit_message>
Check DB if needed, random phone number generator, pre-process for http url.
</commit_message>
<xml_diff>
--- a/api/testData/api_test_cases_single.xlsx
+++ b/api/testData/api_test_cases_single.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cowry\Desktop\fastapi\autotestgit\api\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962F73C2-28CC-43D5-AC3D-EF493E7A2B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4811EEC-730F-4D49-A086-174C1BDB0A86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4830" yWindow="1605" windowWidth="16740" windowHeight="8805" xr2:uid="{EFBB3CF1-3761-4F64-9C29-7999EAF6939F}"/>
+    <workbookView xWindow="2205" yWindow="2070" windowWidth="16740" windowHeight="8805" xr2:uid="{EFBB3CF1-3761-4F64-9C29-7999EAF6939F}"/>
   </bookViews>
   <sheets>
     <sheet name="register" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="47">
   <si>
     <t>method</t>
   </si>
@@ -54,9 +54,6 @@
     <t>request_data</t>
   </si>
   <si>
-    <t>expected_data</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -117,67 +114,76 @@
     <t>register failed password characters does not match rules n</t>
   </si>
   <si>
-    <t>login successfully username password</t>
+    <t>{"username": "aaaaaa", "password": "qqqqqqqq"}</t>
+  </si>
+  <si>
+    <t>{"username": "", "password": "qqqqqqqq"}</t>
+  </si>
+  <si>
+    <t>{"username": "aaaaaa", "password": ""}</t>
+  </si>
+  <si>
+    <t>{"username": "aaa", "password": "qqqqqqqq"}</t>
+  </si>
+  <si>
+    <t>{"username": "aaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa", "password": "qqqqqqqq"}</t>
+  </si>
+  <si>
+    <t>{"username": "aaaaaa", "password": "qqqqqq"}</t>
+  </si>
+  <si>
+    <t>{"refresh":"eyJ0eXAiOiJKV1QiLCJhbGciZu85ABiE", "access":"ZTBiMTk2IMiOze6UY"}</t>
+  </si>
+  <si>
+    <t>{"detail":"No active account found with the given credentials"}</t>
+  </si>
+  <si>
+    <t>expected</t>
+  </si>
+  <si>
+    <t>{"username": "aaaaaa", "passwo": "qqqqqqqq"}</t>
+  </si>
+  <si>
+    <t>{"username": "aaaaaa", "password": "qqqqq"}</t>
+  </si>
+  <si>
+    <t>{"username": "aaaaaa", "password": "qqqq"}</t>
+  </si>
+  <si>
+    <t>check_db_sql</t>
+  </si>
+  <si>
+    <t>select * from tb_users where username='aaaaaa'</t>
+  </si>
+  <si>
+    <t>login pass, username, password</t>
+  </si>
+  <si>
+    <t>{"refresh":"#refresh_token#", "access":"#access_token"}</t>
   </si>
   <si>
     <t>login failed no username</t>
   </si>
   <si>
-    <t>login failed username short than 4 characters</t>
-  </si>
-  <si>
-    <t>login failed username more than 50 characters</t>
-  </si>
-  <si>
-    <t>login failed password short than 8 characters</t>
-  </si>
-  <si>
-    <t>login failed password more than 50 characters</t>
-  </si>
-  <si>
     <t>login failed no password</t>
   </si>
   <si>
-    <t>http://www.alex-info.ca:8000/paymall_admin/authorizations/</t>
-  </si>
-  <si>
-    <t>{"username": "aaaaaa", "password": "qqqqqqqq"}</t>
-  </si>
-  <si>
-    <t>{"username": "", "password": "qqqqqqqq"}</t>
-  </si>
-  <si>
-    <t>{"username": "aaaaaa", "password": ""}</t>
-  </si>
-  <si>
-    <t>{"username": "aaa", "password": "qqqqqqqq"}</t>
-  </si>
-  <si>
-    <t>{"username": "aaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa", "password": "qqqqqqqq"}</t>
-  </si>
-  <si>
-    <t>{"username": "aaaaaa", "password": "qqqqqq"}</t>
-  </si>
-  <si>
-    <t>{"username": "aaaaaa", "password": "qqqqqqqqqqqqqqqqqqqqqqqqqqqqqqqqqqqqqqqqqqqqqqqqqqqqqqqq"}</t>
-  </si>
-  <si>
-    <t>{"refresh":"eyJ0eXAiOiJKV1QiLCJhbGciZu85ABiE", "access":"ZTBiMTk2IMiOze6UY"}</t>
-  </si>
-  <si>
-    <t>{"detail":"No active account found with the given credentials"}</t>
-  </si>
-  <si>
-    <t>expected</t>
-  </si>
-  <si>
-    <t>{"username": "aaaaaa", "passwo": "qqqqqqqq"}</t>
-  </si>
-  <si>
-    <t>{"username": "aaaaaa", "password": "qqqqq"}</t>
-  </si>
-  <si>
-    <t>{"username": "aaaaaa", "password": "qqqq"}</t>
+    <t>{"username": "aaa", "password": ""}</t>
+  </si>
+  <si>
+    <t>login failed wrong username password</t>
+  </si>
+  <si>
+    <t>{'username': ['This field may not be blank.']}</t>
+  </si>
+  <si>
+    <t>{"username": "aa", "password": "bbqqq"}</t>
+  </si>
+  <si>
+    <t>{'password': ['This field may not be blank.']}</t>
+  </si>
+  <si>
+    <t>/paymall_admin/authorizations/</t>
   </si>
 </sst>
 </file>
@@ -214,12 +220,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,26 +537,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA226EC8-69BF-4338-AEC9-E24BC31576C9}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="44.140625" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" customWidth="1"/>
+    <col min="5" max="5" width="31.140625" customWidth="1"/>
+    <col min="6" max="6" width="61.28515625" customWidth="1"/>
+    <col min="7" max="7" width="55.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -565,307 +570,313 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="75">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="F8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="F10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="F11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="F12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="F13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="F14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E15" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="F15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E16" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="F16" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -873,19 +884,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E17" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="F17" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -893,50 +904,52 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E18" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="F18" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4397D820-6F26-498D-BEF6-02BCB312902E}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" customWidth="1"/>
-    <col min="4" max="4" width="49.42578125" customWidth="1"/>
-    <col min="5" max="5" width="47.5703125" customWidth="1"/>
-    <col min="6" max="6" width="52.85546875" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" customWidth="1"/>
+    <col min="5" max="5" width="37.85546875" customWidth="1"/>
+    <col min="6" max="6" width="57.5703125" customWidth="1"/>
+    <col min="7" max="7" width="46.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -948,126 +961,90 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>44</v>
+      </c>
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" t="s">
-        <v>38</v>
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bugs in case running.
</commit_message>
<xml_diff>
--- a/api/testData/api_test_cases_single.xlsx
+++ b/api/testData/api_test_cases_single.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cowry\Desktop\fastapi\autotestgit\api\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4811EEC-730F-4D49-A086-174C1BDB0A86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADFCC5D-EB51-49A7-85A3-AF86C34EEC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="2070" windowWidth="16740" windowHeight="8805" xr2:uid="{EFBB3CF1-3761-4F64-9C29-7999EAF6939F}"/>
+    <workbookView xWindow="2205" yWindow="2070" windowWidth="16740" windowHeight="8805" activeTab="1" xr2:uid="{EFBB3CF1-3761-4F64-9C29-7999EAF6939F}"/>
   </bookViews>
   <sheets>
     <sheet name="register" sheetId="1" r:id="rId1"/>
@@ -159,9 +159,6 @@
     <t>login pass, username, password</t>
   </si>
   <si>
-    <t>{"refresh":"#refresh_token#", "access":"#access_token"}</t>
-  </si>
-  <si>
     <t>login failed no username</t>
   </si>
   <si>
@@ -184,6 +181,9 @@
   </si>
   <si>
     <t>/paymall_admin/authorizations/</t>
+  </si>
+  <si>
+    <t>{"refresh":"#refresh_token#", "access":"#access_token#"}</t>
   </si>
 </sst>
 </file>
@@ -539,7 +539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA226EC8-69BF-4338-AEC9-E24BC31576C9}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -587,7 +587,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
         <v>23</v>
@@ -610,7 +610,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
         <v>24</v>
@@ -630,7 +630,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E4" t="s">
         <v>26</v>
@@ -650,7 +650,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" t="s">
         <v>27</v>
@@ -670,7 +670,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
         <v>25</v>
@@ -690,7 +690,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" t="s">
         <v>33</v>
@@ -710,7 +710,7 @@
         <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E8" t="s">
         <v>33</v>
@@ -730,7 +730,7 @@
         <v>6</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
         <v>34</v>
@@ -750,7 +750,7 @@
         <v>6</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
         <v>34</v>
@@ -770,7 +770,7 @@
         <v>6</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" t="s">
         <v>33</v>
@@ -790,7 +790,7 @@
         <v>6</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E12" t="s">
         <v>28</v>
@@ -810,7 +810,7 @@
         <v>6</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E13" t="s">
         <v>28</v>
@@ -830,7 +830,7 @@
         <v>6</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E14" t="s">
         <v>28</v>
@@ -850,7 +850,7 @@
         <v>6</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E15" t="s">
         <v>28</v>
@@ -870,7 +870,7 @@
         <v>6</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E16" t="s">
         <v>28</v>
@@ -890,7 +890,7 @@
         <v>6</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E17" t="s">
         <v>28</v>
@@ -910,7 +910,7 @@
         <v>6</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E18" t="s">
         <v>32</v>
@@ -929,8 +929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4397D820-6F26-498D-BEF6-02BCB312902E}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -978,13 +978,13 @@
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
         <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -992,16 +992,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s">
         <v>30</v>
@@ -1012,19 +1012,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E4" t="s">
         <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1032,19 +1032,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" t="s">
         <v>40</v>
       </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" t="s">
-        <v>41</v>
-      </c>
       <c r="F5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
API add users and relative handlers.
</commit_message>
<xml_diff>
--- a/api/testData/api_test_cases_single.xlsx
+++ b/api/testData/api_test_cases_single.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cowry\Desktop\fastapi\autotestgit\api\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADFCC5D-EB51-49A7-85A3-AF86C34EEC43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F9F2E0-A7F8-4A99-8911-5D97C57BF81B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="2070" windowWidth="16740" windowHeight="8805" activeTab="1" xr2:uid="{EFBB3CF1-3761-4F64-9C29-7999EAF6939F}"/>
+    <workbookView xWindow="1185" yWindow="4080" windowWidth="21510" windowHeight="8805" activeTab="3" xr2:uid="{EFBB3CF1-3761-4F64-9C29-7999EAF6939F}"/>
   </bookViews>
   <sheets>
     <sheet name="register" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="70">
   <si>
     <t>method</t>
   </si>
@@ -184,6 +184,75 @@
   </si>
   <si>
     <t>{"refresh":"#refresh_token#", "access":"#access_token#"}</t>
+  </si>
+  <si>
+    <t>case_id</t>
+  </si>
+  <si>
+    <t>interface</t>
+  </si>
+  <si>
+    <t>add user</t>
+  </si>
+  <si>
+    <t>user added successfully</t>
+  </si>
+  <si>
+    <t>/paymall_admin/users/</t>
+  </si>
+  <si>
+    <t>failed, user exist</t>
+  </si>
+  <si>
+    <t>failed, mobile phone exist</t>
+  </si>
+  <si>
+    <t>{"username":["A user with that username already exists."]}</t>
+  </si>
+  <si>
+    <t>select * from tb_users WHERE user='#username#'</t>
+  </si>
+  <si>
+    <t>{"mobile":["user with this Mobile Phone number already exists."]}</t>
+  </si>
+  <si>
+    <t>failed, phone number blank</t>
+  </si>
+  <si>
+    <t>failed, user name blank</t>
+  </si>
+  <si>
+    <t>failed, password blank</t>
+  </si>
+  <si>
+    <t>{"username":"#username#","mobile":"#phone#","password":"#password#","email":"a@a.com"}</t>
+  </si>
+  <si>
+    <t>{"id":#id#,"username":"#username#","mobile":"#phone#","email":"a@a.com"}</t>
+  </si>
+  <si>
+    <t>{"username":"","mobile":"#phone#","password":"#password#","email":"a@a.com"}</t>
+  </si>
+  <si>
+    <t>{"username":"#username#","mobile":"","password":"#password#","email":"a@a.com"}</t>
+  </si>
+  <si>
+    <t>{"username":"#username#","mobile":"#phone#","password":"","email":"a@a.com"}</t>
+  </si>
+  <si>
+    <t>{"username":"aaaaaa","mobile":"#phone#","password":"#password#","email":"a@a.com"}</t>
+  </si>
+  <si>
+    <t>{"username":"#username#","mobile":"13111111111","password":"#password#","email":"a@a.com"}</t>
+  </si>
+  <si>
+    <t>{"username": ["This field may not be blank."]}</t>
+  </si>
+  <si>
+    <t>{"mobile": ["This field may not be blank."]}</t>
+  </si>
+  <si>
+    <t>{"password": ["This field may not be blank."]}</t>
   </si>
 </sst>
 </file>
@@ -929,8 +998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4397D820-6F26-498D-BEF6-02BCB312902E}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1068,12 +1137,191 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5572DB7A-BA47-4258-97A3-11C42751545C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="6" max="6" width="53.85546875" customWidth="1"/>
+    <col min="7" max="7" width="62.140625" customWidth="1"/>
+    <col min="8" max="8" width="39.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>